<commit_message>
Sale Schedule Chnages (Dharmee)
</commit_message>
<xml_diff>
--- a/eTactWeb/wwwroot/Uploads/PLAN.xlsx
+++ b/eTactWeb/wwwroot/Uploads/PLAN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soumitra\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C77A1EC-6756-4607-81A9-6EA040E5444E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2304A7D-3CA4-4E8A-88B2-4B09F4099124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>FGHU00005</t>
   </si>
   <si>
-    <t>FGFG00001</t>
-  </si>
-  <si>
     <t>FGSU00001</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>FGAL00003</t>
+  </si>
+  <si>
+    <t>FGFG00001</t>
   </si>
 </sst>
 </file>
@@ -541,13 +541,13 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:AD11"/>
+  <dimension ref="A1:AD14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -747,7 +747,7 @@
     </row>
     <row r="4" spans="1:30" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -783,7 +783,7 @@
     </row>
     <row r="5" spans="1:30" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -819,7 +819,7 @@
     </row>
     <row r="6" spans="1:30" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6">
@@ -869,7 +869,7 @@
     </row>
     <row r="7" spans="1:30" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -909,7 +909,7 @@
     </row>
     <row r="8" spans="1:30" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -945,7 +945,7 @@
     </row>
     <row r="9" spans="1:30" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="11" spans="1:30" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1069,6 +1069,99 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AD11" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD11">
@@ -1078,15 +1171,13 @@
     <cfRule type="duplicateValues" dxfId="5" priority="492"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A11">
-    <cfRule type="duplicateValues" dxfId="4" priority="4492"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4498"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4499"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4500"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="4501"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A11">
-    <cfRule type="duplicateValues" dxfId="3" priority="4493"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="4494"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="4495"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="0" priority="4497"/>
+  <conditionalFormatting sqref="A15:A1048576 A1">
+    <cfRule type="duplicateValues" dxfId="0" priority="4502"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>